<commit_message>
Experimenting with laplacian of gaussian... seems like a waste of time?
</commit_message>
<xml_diff>
--- a/beta_bruteforce_with_norms.xlsx
+++ b/beta_bruteforce_with_norms.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arc\AppData\Local\Temp\scp15596\home\arc\Desktop\supy-res-imaging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arc\AppData\Local\Temp\scp20027\home\arc\Desktop\supy-res-imaging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CE4E18-D02E-419D-ABA0-E93DFBA68FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300E2A36-3C47-477E-9A2E-F9EC19CB818A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RRMSE" sheetId="1" r:id="rId1"/>
@@ -213,6 +213,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -575,8 +576,8 @@
   <dimension ref="A1:AA53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A7" sqref="A7:B7"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented gpu version of SOLE
</commit_message>
<xml_diff>
--- a/beta_bruteforce_with_norms.xlsx
+++ b/beta_bruteforce_with_norms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arc\AppData\Local\Temp\scp20027\home\arc\Desktop\supy-res-imaging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/gb/4_pht1g97qb39ccws84g7d240000gn/T/ch.sudo.cyberduck/81911df4-6c8e-4429-b646-72902ab8f8c0/home/arc/Desktop/supy-res-imaging/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300E2A36-3C47-477E-9A2E-F9EC19CB818A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A77A39-DB8A-FA4C-B01E-0FCCA357627A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="24700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RRMSE" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Beta</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>MAXIMUMS</t>
+  </si>
+  <si>
+    <t>OPTIMAL BETAS</t>
   </si>
 </sst>
 </file>
@@ -573,96 +576,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA53"/>
+  <dimension ref="A1:AA54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A20" sqref="A20"/>
+      <selection pane="topRight" activeCell="AA54" sqref="C54:AA54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="16" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="28" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="16" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="28" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="28" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="16" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="28" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="28" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="16" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="85" max="86" width="26.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -745,7 +747,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -828,7 +830,7 @@
         <v>1.3615273875103031</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.1167798623737652</v>
       </c>
@@ -911,7 +913,7 @@
         <v>1.31998638052224</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.13637536256035551</v>
       </c>
@@ -994,7 +996,7 @@
         <v>1.2740819999622519</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.15925896070970641</v>
       </c>
@@ -1077,7 +1079,7 @@
         <v>1.22407998020324</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.18598239513468401</v>
       </c>
@@ -1160,7 +1162,7 @@
         <v>1.170464392181128</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.2171899850777162</v>
       </c>
@@ -1243,7 +1245,7 @@
         <v>1.144695629289876</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.25363416566335822</v>
       </c>
@@ -1326,7 +1328,7 @@
         <v>1.157324666095793</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.29619362959451739</v>
       </c>
@@ -1409,7 +1411,7 @@
         <v>1.1623879182892369</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.34589451300033741</v>
       </c>
@@ -1492,7 +1494,7 @@
         <v>1.1594270533766211</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.40393513624019939</v>
       </c>
@@ -1575,7 +1577,7 @@
         <v>1.161795231000927</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.47171489618058587</v>
       </c>
@@ -1658,7 +1660,7 @@
         <v>1.182861174294858</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0.55086800655623769</v>
       </c>
@@ -1741,7 +1743,7 @@
         <v>1.1959431647442551</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.64330289991747847</v>
       </c>
@@ -1824,7 +1826,7 @@
         <v>1.2003751562817091</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.75124824117007183</v>
       </c>
@@ -1907,7 +1909,7 @@
         <v>1.1957746250222161</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.87730666212374175</v>
       </c>
@@ -1990,7 +1992,7 @@
         <v>1.18189555994364</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1.0245175126239789</v>
       </c>
@@ -2073,7 +2075,7 @@
         <v>1.185448237583671</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1.196430141237405</v>
       </c>
@@ -2156,12 +2158,12 @@
         <v>1.1942811485916149</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1.3971894723352869</v>
       </c>
       <c r="B19">
-        <v>89.420120239257813</v>
+        <v>89.420120239257812</v>
       </c>
       <c r="C19">
         <v>0.52969855701666857</v>
@@ -2239,7 +2241,7 @@
         <v>1.193623524373927</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1.6316359428938849</v>
       </c>
@@ -2322,7 +2324,7 @@
         <v>1.1834608103027371</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1.9054222085523651</v>
       </c>
@@ -2405,7 +2407,7 @@
         <v>1.17262966584321</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2.2251494327866088</v>
       </c>
@@ -2488,7 +2490,7 @@
         <v>1.1748047493299869</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2.598526445218821</v>
       </c>
@@ -2571,7 +2573,7 @@
         <v>1.1712210279033901</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3.0345556064724311</v>
       </c>
@@ -2654,7 +2656,7 @@
         <v>1.182787609479965</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3.543749860893882</v>
       </c>
@@ -2737,12 +2739,12 @@
         <v>1.1875220602063741</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4.1383862104223734</v>
       </c>
       <c r="B26">
-        <v>264.85671997070313</v>
+        <v>264.85671997070312</v>
       </c>
       <c r="C26">
         <v>0.60532599365039919</v>
@@ -2820,7 +2822,7 @@
         <v>1.2022072133386741</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4.832801721026124</v>
       </c>
@@ -2903,7 +2905,7 @@
         <v>1.2092945505100801</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>5.6437391986112626</v>
       </c>
@@ -2986,7 +2988,7 @@
         <v>1.2190076760355339</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>6.5907508688724734</v>
       </c>
@@ -3069,7 +3071,7 @@
         <v>1.2426307638716829</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>7.6966697940670121</v>
       </c>
@@ -3152,7 +3154,7 @@
         <v>1.2568591718198781</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>8.9881603928746134</v>
       </c>
@@ -3235,7 +3237,7 @@
         <v>1.2674817881887599</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>10.496361336732249</v>
       </c>
@@ -3318,7 +3320,7 @@
         <v>1.2715315489907879</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>12.257636323289031</v>
       </c>
@@ -3401,7 +3403,7 @@
         <v>1.2847685816488399</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>14.31445082861358</v>
       </c>
@@ -3484,7 +3486,7 @@
         <v>1.2988257448670011</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>16.716395977215232</v>
       </c>
@@ -3567,7 +3569,7 @@
         <v>1.303889487845423</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>19.521384216045568</v>
       </c>
@@ -3650,7 +3652,7 @@
         <v>1.300290128104175</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>22.797045620951941</v>
       </c>
@@ -3733,7 +3735,7 @@
         <v>1.2897763182605591</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>26.622358501432171</v>
       </c>
@@ -3816,7 +3818,7 @@
         <v>1.3149663206211739</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>31.089553618622858</v>
       </c>
@@ -3899,7 +3901,7 @@
         <v>1.3375646737806079</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>36.306337928445721</v>
       </c>
@@ -3982,7 +3984,7 @@
         <v>1.3553345823270091</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>42.398491465793029</v>
       </c>
@@ -4065,7 +4067,7 @@
         <v>1.3678573053017731</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>49.512899982305683</v>
       </c>
@@ -4148,7 +4150,7 @@
         <v>1.3752172738578581</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>57.821096456596592</v>
       </c>
@@ -4231,7 +4233,7 @@
         <v>1.3808155872251531</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>67.523396865015584</v>
       </c>
@@ -4314,7 +4316,7 @@
         <v>1.383401581039073</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>78.853729929056499</v>
       </c>
@@ -4397,7 +4399,7 @@
         <v>1.4109229114774471</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>92.08527728773268</v>
       </c>
@@ -4480,7 +4482,7 @@
         <v>1.4446356332127319</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>107.5370600831143</v>
       </c>
@@ -4563,7 +4565,7 @@
         <v>1.4763769786435139</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>125.5816307658541</v>
       </c>
@@ -4646,7 +4648,7 @@
         <v>1.506692419518036</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>146.6540555750943</v>
       </c>
@@ -4729,7 +4731,7 @@
         <v>1.528614397700927</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>171.26240426614049</v>
       </c>
@@ -4812,7 +4814,7 @@
         <v>1.5517569797775459</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>200</v>
       </c>
@@ -4895,7 +4897,7 @@
         <v>1.5714229742240751</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -4998,6 +5000,86 @@
       <c r="AA53">
         <f t="shared" si="0"/>
         <v>1.144695629289876</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54">
+        <v>1.6316359428938849</v>
+      </c>
+      <c r="D54">
+        <v>1.0245175126239789</v>
+      </c>
+      <c r="E54">
+        <v>4.1383862104223734</v>
+      </c>
+      <c r="F54">
+        <v>10.496361336732249</v>
+      </c>
+      <c r="G54">
+        <v>12.257636323289031</v>
+      </c>
+      <c r="H54">
+        <v>57.821096456596592</v>
+      </c>
+      <c r="I54">
+        <v>67.523396865015584</v>
+      </c>
+      <c r="J54">
+        <v>92.08527728773268</v>
+      </c>
+      <c r="K54">
+        <v>107.5370600831143</v>
+      </c>
+      <c r="L54">
+        <v>0.87730666212374175</v>
+      </c>
+      <c r="M54">
+        <v>0.87730666212374175</v>
+      </c>
+      <c r="N54">
+        <v>0.75124824117007183</v>
+      </c>
+      <c r="O54">
+        <v>0.75124824117007183</v>
+      </c>
+      <c r="P54">
+        <v>0.75124824117007183</v>
+      </c>
+      <c r="Q54">
+        <v>0.64330289991747847</v>
+      </c>
+      <c r="R54">
+        <v>0.64330289991747847</v>
+      </c>
+      <c r="S54">
+        <v>0.55086800655623769</v>
+      </c>
+      <c r="T54">
+        <v>0.55086800655623769</v>
+      </c>
+      <c r="U54">
+        <v>0.55086800655623769</v>
+      </c>
+      <c r="V54">
+        <v>0.55086800655623769</v>
+      </c>
+      <c r="W54">
+        <v>0.47171489618058587</v>
+      </c>
+      <c r="X54">
+        <v>0.25363416566335822</v>
+      </c>
+      <c r="Y54">
+        <v>0.25363416566335822</v>
+      </c>
+      <c r="Z54">
+        <v>0.2171899850777162</v>
+      </c>
+      <c r="AA54">
+        <v>0.2171899850777162</v>
       </c>
     </row>
   </sheetData>
@@ -5014,21 +5096,21 @@
       <selection activeCell="AB49" sqref="AB49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="13" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5111,7 +5193,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -5194,7 +5276,7 @@
         <v>0.43694648291692628</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.1167798623737652</v>
       </c>
@@ -5277,7 +5359,7 @@
         <v>0.44695805566401081</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.13637536256035551</v>
       </c>
@@ -5360,7 +5442,7 @@
         <v>0.45827096812393309</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.15925896070970641</v>
       </c>
@@ -5443,7 +5525,7 @@
         <v>0.47103976605338449</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.18598239513468401</v>
       </c>
@@ -5526,7 +5608,7 @@
         <v>0.4854278129340715</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.2171899850777162</v>
       </c>
@@ -5609,7 +5691,7 @@
         <v>0.49375900515598542</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.25363416566335822</v>
       </c>
@@ -5692,7 +5774,7 @@
         <v>0.49264927536701392</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.29619362959451739</v>
       </c>
@@ -5775,7 +5857,7 @@
         <v>0.49342445039735072</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.34589451300033741</v>
       </c>
@@ -5858,7 +5940,7 @@
         <v>0.49622779375124743</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.40393513624019939</v>
       </c>
@@ -5941,7 +6023,7 @@
         <v>0.49775555505741498</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.47171489618058587</v>
       </c>
@@ -6024,7 +6106,7 @@
         <v>0.49462799301633209</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0.55086800655623769</v>
       </c>
@@ -6107,7 +6189,7 @@
         <v>0.49358686554170178</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.64330289991747847</v>
       </c>
@@ -6190,7 +6272,7 @@
         <v>0.49478746820772429</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.75124824117007183</v>
       </c>
@@ -6273,7 +6355,7 @@
         <v>0.49840398743789138</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.87730666212374175</v>
       </c>
@@ -6356,7 +6438,7 @@
         <v>0.50468312825665262</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1.0245175126239789</v>
       </c>
@@ -6439,7 +6521,7 @@
         <v>0.50655857154710793</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1.196430141237405</v>
       </c>
@@ -6522,12 +6604,12 @@
         <v>0.50711611066234497</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1.3971894723352869</v>
       </c>
       <c r="B19">
-        <v>89.420120239257813</v>
+        <v>89.420120239257812</v>
       </c>
       <c r="C19">
         <v>0.85325526638355342</v>
@@ -6605,7 +6687,7 @@
         <v>0.51038690121661434</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1.6316359428938849</v>
       </c>
@@ -6688,7 +6770,7 @@
         <v>0.51653765860713952</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1.9054222085523651</v>
       </c>
@@ -6771,7 +6853,7 @@
         <v>0.52318277433109861</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2.2251494327866088</v>
       </c>
@@ -6854,7 +6936,7 @@
         <v>0.52606702714672771</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2.598526445218821</v>
       </c>
@@ -6937,7 +7019,7 @@
         <v>0.53067440076003036</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3.0345556064724311</v>
       </c>
@@ -7020,7 +7102,7 @@
         <v>0.5304096189802685</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3.543749860893882</v>
       </c>
@@ -7103,12 +7185,12 @@
         <v>0.53220822415814217</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4.1383862104223734</v>
       </c>
       <c r="B26">
-        <v>264.85671997070313</v>
+        <v>264.85671997070312</v>
       </c>
       <c r="C26">
         <v>0.86588779056083032</v>
@@ -7186,7 +7268,7 @@
         <v>0.53067318292359134</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4.832801721026124</v>
       </c>
@@ -7269,7 +7351,7 @@
         <v>0.53144589909718098</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>5.6437391986112626</v>
       </c>
@@ -7352,7 +7434,7 @@
         <v>0.53124578868590411</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>6.5907508688724734</v>
       </c>
@@ -7435,7 +7517,7 @@
         <v>0.52644363898994617</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>7.6966697940670121</v>
       </c>
@@ -7518,7 +7600,7 @@
         <v>0.52460506428711895</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>8.9881603928746134</v>
       </c>
@@ -7601,7 +7683,7 @@
         <v>0.52388143699279754</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>10.496361336732249</v>
       </c>
@@ -7684,7 +7766,7 @@
         <v>0.52529397906372755</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>12.257636323289031</v>
       </c>
@@ -7767,7 +7849,7 @@
         <v>0.52379626987223504</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>14.31445082861358</v>
       </c>
@@ -7850,7 +7932,7 @@
         <v>0.52212311310893678</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>16.716395977215232</v>
       </c>
@@ -7933,7 +8015,7 @@
         <v>0.52352351135240793</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>19.521384216045568</v>
       </c>
@@ -8016,7 +8098,7 @@
         <v>0.5280548480933599</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>22.797045620951941</v>
       </c>
@@ -8099,7 +8181,7 @@
         <v>0.53542007153077287</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>26.622358501432171</v>
       </c>
@@ -8182,7 +8264,7 @@
         <v>0.53051572323108753</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>31.089553618622858</v>
       </c>
@@ -8265,7 +8347,7 @@
         <v>0.52672676736511703</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>36.306337928445721</v>
       </c>
@@ -8348,7 +8430,7 @@
         <v>0.52454124325224449</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>42.398491465793029</v>
       </c>
@@ -8431,7 +8513,7 @@
         <v>0.52422979415243431</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>49.512899982305683</v>
       </c>
@@ -8514,7 +8596,7 @@
         <v>0.5258997357075198</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>57.821096456596592</v>
       </c>
@@ -8597,7 +8679,7 @@
         <v>0.52842776452832485</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>67.523396865015584</v>
       </c>
@@ -8680,7 +8762,7 @@
         <v>0.53236783501973428</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>78.853729929056499</v>
       </c>
@@ -8763,7 +8845,7 @@
         <v>0.5271442538838127</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>92.08527728773268</v>
       </c>
@@ -8846,7 +8928,7 @@
         <v>0.51984222601682217</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>107.5370600831143</v>
       </c>
@@ -8929,7 +9011,7 @@
         <v>0.51356047045273945</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>125.5816307658541</v>
       </c>
@@ -9012,7 +9094,7 @@
         <v>0.50813029415771827</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>146.6540555750943</v>
       </c>
@@ -9095,7 +9177,7 @@
         <v>0.50620725271570288</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>171.26240426614049</v>
       </c>
@@ -9178,7 +9260,7 @@
         <v>0.50437868412720244</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>200</v>
       </c>
@@ -9261,7 +9343,7 @@
         <v>0.50456419935343078</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>53</v>
       </c>

</xml_diff>